<commit_message>
Max and min in integer
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Camilo Fernandez\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicoquintero/Documents/Probabilidad_y_estadistica_1/Proyecto-Probabilidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8004000A-DEFC-4688-9F62-532E8052CFA2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE8FFAC-6D38-014D-900E-8B2F354F0DD2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2E2781E3-2DED-A446-9797-3F25D4E5CF85}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{2E2781E3-2DED-A446-9797-3F25D4E5CF85}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>2005_1</t>
   </si>
@@ -259,6 +259,12 @@
   </si>
   <si>
     <t>Inflación_COL</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>MAX</t>
   </si>
 </sst>
 </file>
@@ -1923,20 +1929,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE5F1C81-20BB-534E-8414-C24271AE9737}">
   <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.125" customWidth="1"/>
-    <col min="3" max="3" width="21.625" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="6" max="6" width="21.5" customWidth="1"/>
-    <col min="7" max="7" width="23.125" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="4" t="s">
         <v>63</v>
@@ -1963,7 +1969,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1994,7 +2000,7 @@
         <v>5.2366666666666672</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2025,7 +2031,7 @@
         <v>4.96</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -2056,7 +2062,7 @@
         <v>4.9366666666666665</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -2087,7 +2093,7 @@
         <v>5.0733333333333333</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -2118,7 +2124,7 @@
         <v>4.2866666666666662</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -2149,7 +2155,7 @@
         <v>4.0333333333333341</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
@@ -2180,7 +2186,7 @@
         <v>4.54</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
@@ -2211,7 +2217,7 @@
         <v>4.3266666666666671</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
@@ -2242,7 +2248,7 @@
         <v>5.246666666666667</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
@@ -2273,7 +2279,7 @@
         <v>6.1733333333333347</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
@@ -2304,7 +2310,7 @@
         <v>5.333333333333333</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>11</v>
       </c>
@@ -2335,7 +2341,7 @@
         <v>5.4200000000000008</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>12</v>
       </c>
@@ -2366,7 +2372,7 @@
         <v>6.0933333333333337</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>13</v>
       </c>
@@ -2397,7 +2403,7 @@
         <v>6.4333333333333336</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>14</v>
       </c>
@@ -2428,7 +2434,7 @@
         <v>7.6533333333333333</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>15</v>
       </c>
@@ -2459,7 +2465,7 @@
         <v>7.78</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>16</v>
       </c>
@@ -2490,7 +2496,7 @@
         <v>6.5966666666666667</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>17</v>
       </c>
@@ -2521,7 +2527,7 @@
         <v>4.7700000000000005</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
@@ -2552,7 +2558,7 @@
         <v>3.2066666666666666</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>19</v>
       </c>
@@ -2583,7 +2589,7 @@
         <v>2.3633333333333333</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>20</v>
       </c>
@@ -2614,7 +2620,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>21</v>
       </c>
@@ -2645,7 +2651,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>22</v>
       </c>
@@ -2676,7 +2682,7 @@
         <v>2.2766666666666668</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>23</v>
       </c>
@@ -2707,7 +2713,7 @@
         <v>2.6966666666666668</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>24</v>
       </c>
@@ -2738,7 +2744,7 @@
         <v>3.2533333333333334</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>25</v>
       </c>
@@ -2769,7 +2775,7 @@
         <v>3.03</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>26</v>
       </c>
@@ -2800,7 +2806,7 @@
         <v>3.4733333333333332</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>27</v>
       </c>
@@ -2831,7 +2837,7 @@
         <v>3.9033333333333329</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>28</v>
       </c>
@@ -2862,7 +2868,7 @@
         <v>3.4966666666666661</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>29</v>
       </c>
@@ -2893,7 +2899,7 @@
         <v>3.3566666666666669</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>30</v>
       </c>
@@ -2924,7 +2930,7 @@
         <v>3.0733333333333328</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>31</v>
       </c>
@@ -2955,7 +2961,7 @@
         <v>2.7566666666666664</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>32</v>
       </c>
@@ -2986,7 +2992,7 @@
         <v>1.9133333333333333</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>33</v>
       </c>
@@ -3017,7 +3023,7 @@
         <v>2.06</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>34</v>
       </c>
@@ -3048,7 +3054,7 @@
         <v>2.2533333333333334</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>35</v>
       </c>
@@ -3079,7 +3085,7 @@
         <v>1.8466666666666667</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>36</v>
       </c>
@@ -3110,7 +3116,7 @@
         <v>2.3199999999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>37</v>
       </c>
@@ -3141,7 +3147,7 @@
         <v>2.8133333333333339</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>38</v>
       </c>
@@ -3172,7 +3178,7 @@
         <v>2.9233333333333333</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>39</v>
       </c>
@@ -3203,7 +3209,7 @@
         <v>3.5333333333333337</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>40</v>
       </c>
@@ -3234,7 +3240,7 @@
         <v>4.246666666666667</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>41</v>
       </c>
@@ -3265,7 +3271,7 @@
         <v>4.4899999999999993</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>42</v>
       </c>
@@ -3296,7 +3302,7 @@
         <v>4.8500000000000005</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>43</v>
       </c>
@@ -3327,7 +3333,7 @@
         <v>6.3500000000000005</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>44</v>
       </c>
@@ -3358,7 +3364,7 @@
         <v>7.6733333333333329</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>45</v>
       </c>
@@ -3389,7 +3395,7 @@
         <v>8.2433333333333323</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>46</v>
       </c>
@@ -3420,7 +3426,7 @@
         <v>8.1133333333333333</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>47</v>
       </c>
@@ -3451,7 +3457,7 @@
         <v>6.0633333333333335</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>48</v>
       </c>
@@ -3482,7 +3488,7 @@
         <v>5.1133333333333333</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>49</v>
       </c>
@@ -3513,7 +3519,7 @@
         <v>4.34</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>50</v>
       </c>
@@ -3544,7 +3550,7 @@
         <v>3.7466666666666666</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>51</v>
       </c>
@@ -3575,7 +3581,7 @@
         <v>4.0866666666666669</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>52</v>
       </c>
@@ -3606,7 +3612,7 @@
         <v>3.3966666666666665</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>53</v>
       </c>
@@ -3637,7 +3643,7 @@
         <v>3.1633333333333336</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
         <v>54</v>
       </c>
@@ -3668,7 +3674,7 @@
         <v>3.15</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
         <v>55</v>
       </c>
@@ -3699,7 +3705,7 @@
         <v>3.2600000000000002</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
         <v>56</v>
       </c>
@@ -3730,7 +3736,7 @@
         <v>3.1233333333333331</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
         <v>57</v>
       </c>
@@ -3761,7 +3767,7 @@
         <v>3.33</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
         <v>58</v>
       </c>
@@ -3792,7 +3798,7 @@
         <v>3.7866666666666666</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
         <v>59</v>
       </c>
@@ -3823,7 +3829,7 @@
         <v>3.8333333333333335</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
         <v>60</v>
       </c>
@@ -3854,7 +3860,7 @@
         <v>3.7333333333333329</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
         <v>61</v>
       </c>
@@ -3885,7 +3891,7 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
         <v>62</v>
       </c>
@@ -3916,14 +3922,14 @@
         <v>1.9399999999999997</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E65" s="14"/>
       <c r="I65" s="17"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E66" s="14"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="16" t="s">
         <v>69</v>
       </c>
@@ -3960,7 +3966,7 @@
         <v>4.1656613756613767</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="16" t="s">
         <v>70</v>
       </c>
@@ -3969,7 +3975,7 @@
         <v>14032384.024081446</v>
       </c>
       <c r="C68">
-        <f t="shared" ref="C68:I68" si="1">_xlfn.VAR.S(C2:C64)</f>
+        <f t="shared" ref="C68:H68" si="1">_xlfn.VAR.S(C2:C64)</f>
         <v>97334306.961035445</v>
       </c>
       <c r="D68">
@@ -3993,11 +3999,11 @@
         <v>61780652.079428889</v>
       </c>
       <c r="I68">
-        <f t="shared" si="1"/>
+        <f>_xlfn.VAR.S(I2:I64)</f>
         <v>2.746875854810249</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A69" s="16" t="s">
         <v>71</v>
       </c>
@@ -4006,7 +4012,7 @@
         <v>3745.9823843794898</v>
       </c>
       <c r="C69">
-        <f t="shared" ref="C69:I69" si="2">_xlfn.STDEV.S(C2:C64)</f>
+        <f t="shared" ref="C69:H69" si="2">_xlfn.STDEV.S(C2:C64)</f>
         <v>9865.815068256421</v>
       </c>
       <c r="D69">
@@ -4030,44 +4036,112 @@
         <v>7860.0669258873932</v>
       </c>
       <c r="I69">
-        <f t="shared" si="2"/>
+        <f>_xlfn.STDEV.S(I2:I64)</f>
         <v>1.6573701622782548</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E70" s="14"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E71" s="14"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B70" s="15">
+        <f>MIN(B2:B64)</f>
+        <v>19854.275258932787</v>
+      </c>
+      <c r="C70" s="15">
+        <f t="shared" ref="C70:I70" si="3">MIN(C2:C64)</f>
+        <v>17216.113283945448</v>
+      </c>
+      <c r="D70" s="15">
+        <f t="shared" si="3"/>
+        <v>119348.21424077044</v>
+      </c>
+      <c r="E70" s="15">
+        <f t="shared" si="3"/>
+        <v>8.014970827520612</v>
+      </c>
+      <c r="F70" s="15">
+        <f t="shared" si="3"/>
+        <v>638.59567633333336</v>
+      </c>
+      <c r="G70" s="15">
+        <f t="shared" si="3"/>
+        <v>430.23108500000006</v>
+      </c>
+      <c r="H70" s="15">
+        <f t="shared" si="3"/>
+        <v>38284.011000047001</v>
+      </c>
+      <c r="I70" s="15">
+        <f t="shared" si="3"/>
+        <v>1.8466666666666667</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B71" s="15">
+        <f>MAX(B2:B64)</f>
+        <v>35248.099226554572</v>
+      </c>
+      <c r="C71" s="15">
+        <f t="shared" ref="C71:I71" si="4">MAX(C2:C64)</f>
+        <v>52595.955187872787</v>
+      </c>
+      <c r="D71" s="15">
+        <f t="shared" si="4"/>
+        <v>241371.21655283868</v>
+      </c>
+      <c r="E71" s="15">
+        <f t="shared" si="4"/>
+        <v>20.334270249933372</v>
+      </c>
+      <c r="F71" s="15">
+        <f t="shared" si="4"/>
+        <v>2203.4850303333333</v>
+      </c>
+      <c r="G71" s="15">
+        <f t="shared" si="4"/>
+        <v>1756.5150223333333</v>
+      </c>
+      <c r="H71" s="15">
+        <f t="shared" si="4"/>
+        <v>65242.181999938795</v>
+      </c>
+      <c r="I71" s="15">
+        <f t="shared" si="4"/>
+        <v>8.2433333333333323</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E72" s="14"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E73" s="14"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E74" s="14"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E75" s="14"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E76" s="14"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E77" s="14"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E78" s="14"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E79" s="14"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E80" s="14"/>
     </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E81" s="13"/>
     </row>
   </sheetData>

</xml_diff>